<commit_message>
ok it synced. Still an issue with questions without a destination
</commit_message>
<xml_diff>
--- a/appcode/Hackathon Question 1.xlsx
+++ b/appcode/Hackathon Question 1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Are you seeking light entertainment, or do you want to feel something?</t>
   </si>
   <si>
-    <t>PK</t>
-  </si>
-  <si>
     <t>Old question</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>Yeah!</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>Not even once</t>
@@ -271,26 +265,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6760563380282"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1596244131455"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.5023474178404"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.3380281690141"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1596244131455"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6760563380282"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.3333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6760563380282"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5023474178404"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3380281690141"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.1596244131455"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6760563380282"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.3333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6760563380282"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -301,7 +295,7 @@
       <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -309,7 +303,7 @@
       <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -317,7 +311,7 @@
       <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -325,7 +319,7 @@
       <c r="B5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -333,7 +327,7 @@
       <c r="B6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -341,7 +335,7 @@
       <c r="B7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -349,7 +343,7 @@
       <c r="B8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
     </row>
@@ -357,7 +351,7 @@
       <c r="B9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
     </row>
@@ -371,475 +365,334 @@
       <c r="E19" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>24</v>
+        <v>3</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E30" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>32</v>
+      <c r="E30" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E35" s="0" t="n">
         <v>6</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E36" s="0" t="n">
         <v>6</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>